<commit_message>
Updated per additional development.
</commit_message>
<xml_diff>
--- a/Constellations.xlsx
+++ b/Constellations.xlsx
@@ -1923,7 +1923,7 @@
     <t>α-Vul</t>
   </si>
   <si>
-    <t>CONSTELLATION DATA (as of 10-Sep-2024 @ 06:13 PM) (88 Constellations)</t>
+    <t>CONSTELLATION DATA (as of 11-Sep-2024 @ 02:10 PM) (88 Constellations)</t>
   </si>
 </sst>
 </file>
@@ -4827,7 +4827,7 @@
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape"/>
   <headerFooter>
-    <oddFooter>Data courtesy of: 1) Skyfield, 2) © Dominic Ford 2011–2024.; Maps: GO ASTRONOMY © 2024
+    <oddFooter>Data courtesy of: 1) Skyfield, 2) © Dominic Ford 2011–2024; Maps: GO ASTRONOMY © 2024
 &amp;CFile Name: &amp;F
 &amp;CPage &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>